<commit_message>
ci: update ia forms
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Cote d'Ivoire/civ_oncho_ia_202309_1_site.xlsx
+++ b/ONCHO/Impact Assessments/Cote d'Ivoire/civ_oncho_ia_202309_1_site.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Cote d'Ivoire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F50F081-99F9-49C4-8D3C-1CCECA7B3AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F993DB47-BD35-40E6-8C15-413C0E20015F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="282">
   <si>
     <t>type</t>
   </si>
@@ -886,6 +886,9 @@
   </si>
   <si>
     <t>civ_oncho_ia_202309_1_site</t>
+  </si>
+  <si>
+    <t>M.BORLA DIOULASSO</t>
   </si>
 </sst>
 </file>
@@ -2028,8 +2031,8 @@
   <dimension ref="A1:G191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A141" sqref="A141:XFD143"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3202,13 +3205,13 @@
         <v>42</v>
       </c>
       <c r="B97" s="26" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
       <c r="C97" s="26" t="s">
         <v>123</v>
       </c>
       <c r="F97" s="26" t="s">
-        <v>79</v>
+        <v>224</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -3888,7 +3891,7 @@
         <v>106</v>
       </c>
       <c r="G146" s="26" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -4256,7 +4259,7 @@
         <v>224</v>
       </c>
       <c r="G172" s="26" t="s">
-        <v>123</v>
+        <v>281</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -4792,7 +4795,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="26" customFormat="1" ht="31.5">
+    <row r="3" spans="1:24" s="26" customFormat="1" ht="30">
       <c r="A3" s="15" t="s">
         <v>116</v>
       </c>

</xml_diff>